<commit_message>
hastar only in progress
</commit_message>
<xml_diff>
--- a/log/data_2o1r.xlsx
+++ b/log/data_2o1r.xlsx
@@ -506,17 +506,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.021382</t>
+          <t>0.00162</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>9.6e-05</t>
+          <t>8.2e-05</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.573133</t>
+          <t>0.004396</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -526,12 +526,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.596686</t>
+          <t>0.007247</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>5.4e-05</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.002126</t>
+          <t>0.001551</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.000103</t>
+          <t>8.7e-05</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.4137</t>
+          <t>0.005924</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -583,12 +583,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.417172</t>
+          <t>0.008699</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -620,17 +620,17 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.00245</t>
+          <t>0.001693</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>9.8e-05</t>
+          <t>8.7e-05</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.508275</t>
+          <t>0.003071</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -640,12 +640,12 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.512804</t>
+          <t>0.006026</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>3e-05</t>
+          <t>3.7e-05</t>
         </is>
       </c>
     </row>
@@ -677,17 +677,17 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.00271701</t>
+          <t>0.001604</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>9.1e-05</t>
+          <t>9e-05</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.393928</t>
+          <t>0.006222</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -697,12 +697,12 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.398729</t>
+          <t>0.00906</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>4.1e-05</t>
+          <t>4.7e-05</t>
         </is>
       </c>
     </row>
@@ -734,17 +734,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.002317</t>
+          <t>0.001607</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.000104</t>
+          <t>8.9e-05</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.462719</t>
+          <t>0.00526</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -754,12 +754,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.467022</t>
+          <t>0.008106</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>3.5e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -791,17 +791,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.00278901</t>
+          <t>0.001624</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>0.000101</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.48361</t>
+          <t>0.00486</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -811,12 +811,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.488471</t>
+          <t>0.007723</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>4.4e-05</t>
+          <t>4.6e-05</t>
         </is>
       </c>
     </row>
@@ -833,32 +833,28 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>F</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>b3,b1</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.002224</t>
+          <t>0.001261</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.000102</t>
+          <t>8.4e-05</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.583529</t>
+          <t>0.0022</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -868,12 +864,12 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.588014</t>
+          <t>0.004609</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.000155</t>
+          <t>1.9e-05</t>
         </is>
       </c>
     </row>
@@ -905,17 +901,17 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.00258401</t>
+          <t>0.001716</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>9.9e-05</t>
+          <t>8.3e-05</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.537088</t>
+          <t>0.001644</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -925,12 +921,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.541704</t>
+          <t>0.004631</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>3.3e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -962,17 +958,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0.00273801</t>
+          <t>0.001615</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>9.1e-05</t>
+          <t>8.6e-05</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.523292</t>
+          <t>0.003736</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -982,12 +978,12 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.527992</t>
+          <t>0.006569</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.5e-05</t>
         </is>
       </c>
     </row>
@@ -1019,17 +1015,17 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0.002164</t>
+          <t>0.001609</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>8e-05</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.454888</t>
+          <t>0.00214</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1039,12 +1035,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.458964</t>
+          <t>0.004966</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>3.3e-05</t>
+          <t>3.6e-05</t>
         </is>
       </c>
     </row>
@@ -1076,17 +1072,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0.002227</t>
+          <t>0.001649</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>9.1e-05</t>
+          <t>8.5e-05</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.51708</t>
+          <t>0.002437</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1096,12 +1092,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0.521279</t>
+          <t>0.005339</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>3.8e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -1133,17 +1129,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0.00240601</t>
+          <t>0.001564</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>8.7e-05</t>
+          <t>8.1e-05</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0.274196</t>
+          <t>0.001764</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1153,12 +1149,12 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0.278619</t>
+          <t>0.004609</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>5e-05</t>
+          <t>4.5e-05</t>
         </is>
       </c>
     </row>
@@ -1190,17 +1186,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0.00242</t>
+          <t>0.001674</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>9.3e-05</t>
+          <t>8.3e-05</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.510859</t>
+          <t>0.002781</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1210,12 +1206,12 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0.5153</t>
+          <t>0.005709</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>3e-05</t>
+          <t>3.6e-05</t>
         </is>
       </c>
     </row>
@@ -1247,17 +1243,17 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0.002196</t>
+          <t>0.001625</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>9.2e-05</t>
+          <t>9.4e-05</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0.374583</t>
+          <t>0.004436</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1267,12 +1263,12 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.378722</t>
+          <t>0.007311</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>3.5e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -1304,17 +1300,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0.00233</t>
+          <t>0.001547</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>8.4e-05</t>
+          <t>7.8e-05</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.320374</t>
+          <t>0.001895</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1324,12 +1320,12 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.324609</t>
+          <t>0.004628</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>4.4e-05</t>
         </is>
       </c>
     </row>
@@ -1361,17 +1357,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0.002348</t>
+          <t>0.001638</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>9.7e-05</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0.53717</t>
+          <t>0.003375</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1381,7 +1377,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.541525</t>
+          <t>0.006287</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1418,17 +1414,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0.00278301</t>
+          <t>0.001601</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>9.2e-05</t>
+          <t>7.9e-05</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0.419271</t>
+          <t>0.001731</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1438,12 +1434,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.42402</t>
+          <t>0.004503</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>5e-05</t>
         </is>
       </c>
     </row>
@@ -1475,17 +1471,17 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0.002416</t>
+          <t>0.001565</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>9.7e-05</t>
+          <t>9e-05</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0.317501</t>
+          <t>0.00236</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1495,12 +1491,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>0.321882</t>
+          <t>0.005162</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>4.6e-05</t>
         </is>
       </c>
     </row>
@@ -1532,17 +1528,17 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0.00266801</t>
+          <t>0.001648</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0.000111</t>
+          <t>7.9e-05</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0.417347</t>
+          <t>0.002897</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1552,12 +1548,12 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>0.422094</t>
+          <t>0.005768</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.4e-05</t>
         </is>
       </c>
     </row>
@@ -1589,17 +1585,17 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0.002474</t>
+          <t>0.001706</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0.000114</t>
+          <t>8.3e-05</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0.58215</t>
+          <t>0.003534</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1609,12 +1605,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0.586716</t>
+          <t>0.006481</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>3.8e-05</t>
+          <t>3.7e-05</t>
         </is>
       </c>
     </row>
@@ -1646,17 +1642,17 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0.00283201</t>
+          <t>0.00161</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0.000115</t>
+          <t>8e-05</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0.49758</t>
+          <t>0.00354</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1666,12 +1662,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0.502549</t>
+          <t>0.00635</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>4.2e-05</t>
+          <t>4.3e-05</t>
         </is>
       </c>
     </row>
@@ -1703,17 +1699,17 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0.00243501</t>
+          <t>0.001679</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0.000118</t>
+          <t>7.9e-05</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>0.51046</t>
+          <t>0.001957</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1723,12 +1719,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>0.514979</t>
+          <t>0.004869</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>3.4e-05</t>
+          <t>3.5e-05</t>
         </is>
       </c>
     </row>
@@ -1760,17 +1756,17 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0.00270601</t>
+          <t>0.001761</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0.000103</t>
+          <t>9.2e-05</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>0.428917</t>
+          <t>0.00334</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1780,12 +1776,12 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>0.433667</t>
+          <t>0.006321</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>3.2e-05</t>
+          <t>3.7e-05</t>
         </is>
       </c>
     </row>
@@ -1802,7 +1798,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>F</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1810,24 +1806,20 @@
           <t>0</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>b3,b1</t>
-        </is>
-      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0.002387</t>
+          <t>0.001257</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>9.6e-05</t>
+          <t>7.6e-05</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0.553039</t>
+          <t>0.002694</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1837,12 +1829,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>0.557633</t>
+          <t>0.005089</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>8.3e-05</t>
+          <t>2.4e-05</t>
         </is>
       </c>
     </row>
@@ -1874,17 +1866,17 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0.00241</t>
+          <t>0.001377</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>9.8e-05</t>
+          <t>8.5e-05</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>0.513693</t>
+          <t>0.005761</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1894,12 +1886,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>0.518646</t>
+          <t>0.008358</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>0.000201</t>
+          <t>4.7e-05</t>
         </is>
       </c>
     </row>
@@ -1931,17 +1923,17 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0.00270701</t>
+          <t>0.00169</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>9.1e-05</t>
+          <t>7.4e-05</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>0.405144</t>
+          <t>0.002552</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1951,12 +1943,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>0.409882</t>
+          <t>0.00544</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.3e-05</t>
         </is>
       </c>
     </row>
@@ -1988,17 +1980,17 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0.00301301</t>
+          <t>0.003204</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0.000103</t>
+          <t>0.000145</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>0.459216</t>
+          <t>0.004096</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2008,12 +2000,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>0.464308</t>
+          <t>0.009201</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>4.3e-05</t>
+          <t>6.3e-05</t>
         </is>
       </c>
     </row>
@@ -2045,17 +2037,17 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0.00247</t>
+          <t>0.001692</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0.000104</t>
+          <t>7.6e-05</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>0.543537</t>
+          <t>0.001886</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2065,12 +2057,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>0.548053</t>
+          <t>0.004816</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>4e-05</t>
+          <t>3.4e-05</t>
         </is>
       </c>
     </row>
@@ -2102,17 +2094,17 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>0.00239</t>
+          <t>0.001723</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>0.000101</t>
+          <t>8.8e-05</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>0.53497</t>
+          <t>0.003612</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2122,12 +2114,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>0.539345</t>
+          <t>0.006611</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>3.3e-05</t>
+          <t>3.9e-05</t>
         </is>
       </c>
     </row>
@@ -2159,17 +2151,17 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>0.002315</t>
+          <t>0.001668</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>9.6e-05</t>
+          <t>8e-05</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>0.469668</t>
+          <t>0.000996</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2179,12 +2171,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>0.474103</t>
+          <t>0.00386</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.6e-05</t>
         </is>
       </c>
     </row>
@@ -2216,17 +2208,17 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>0.00283501</t>
+          <t>0.001738</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>8.2e-05</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>0.428698</t>
+          <t>0.001383</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2236,12 +2228,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>0.433618</t>
+          <t>0.004354</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>3.3e-05</t>
+          <t>3.5e-05</t>
         </is>
       </c>
     </row>
@@ -2273,17 +2265,17 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>0.00238001</t>
+          <t>0.001549</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>9.3e-05</t>
+          <t>7.5e-05</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>0.261382</t>
+          <t>0.001007</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2293,12 +2285,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>0.265776</t>
+          <t>0.003732</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>4e-05</t>
         </is>
       </c>
     </row>
@@ -2330,17 +2322,17 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0.00274901</t>
+          <t>0.001695</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>9.5e-05</t>
+          <t>7.8e-05</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>0.467497</t>
+          <t>0.000987</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2350,12 +2342,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>0.472272</t>
+          <t>0.003923</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.5e-05</t>
         </is>
       </c>
     </row>
@@ -2387,17 +2379,17 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>0.002425</t>
+          <t>0.001634</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>9.7e-05</t>
+          <t>8.3e-05</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>0.326769</t>
+          <t>0.002417</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2407,12 +2399,12 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>0.33114</t>
+          <t>0.00525</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.6e-05</t>
         </is>
       </c>
     </row>
@@ -2444,17 +2436,17 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>0.00232</t>
+          <t>0.00163</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>9.5e-05</t>
+          <t>8.3e-05</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>0.513229</t>
+          <t>0.005411</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2464,12 +2456,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>0.517523</t>
+          <t>0.008286</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -2501,17 +2493,17 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>0.002347</t>
+          <t>0.00169</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>8.3e-05</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>0.451958</t>
+          <t>0.005223</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2521,12 +2513,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>0.456306</t>
+          <t>0.00815</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>3.8e-05</t>
         </is>
       </c>
     </row>
@@ -2558,17 +2550,17 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>0.00272401</t>
+          <t>0.001597</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>9.3e-05</t>
+          <t>8.1e-05</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>0.437626</t>
+          <t>0.001472</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -2578,12 +2570,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>0.442332</t>
+          <t>0.004276</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>3.8e-05</t>
+          <t>4.5e-05</t>
         </is>
       </c>
     </row>
@@ -2615,17 +2607,17 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>0.00260601</t>
+          <t>0.001714</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>9.2e-05</t>
+          <t>7.8e-05</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>0.420081</t>
+          <t>0.00251</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2635,12 +2627,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>0.424655</t>
+          <t>0.005423</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>3.2e-05</t>
+          <t>3.9e-05</t>
         </is>
       </c>
     </row>
@@ -2672,17 +2664,17 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>0.00233</t>
+          <t>0.001722</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>9.2e-05</t>
+          <t>7.8e-05</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>0.429061</t>
+          <t>0.002512</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2692,12 +2684,12 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>0.433386</t>
+          <t>0.005502</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>3.3e-05</t>
+          <t>3.5e-05</t>
         </is>
       </c>
     </row>
@@ -2729,17 +2721,17 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0.002323</t>
+          <t>0.001716</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>9.9e-05</t>
+          <t>8.5e-05</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>0.568191</t>
+          <t>0.002637</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2749,12 +2741,12 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>0.57249</t>
+          <t>0.0056</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>3.3e-05</t>
+          <t>3.7e-05</t>
         </is>
       </c>
     </row>
@@ -2771,32 +2763,28 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>F</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>b3,b1</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0.002258</t>
+          <t>0.001255</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>9.5e-05</t>
+          <t>8.7e-05</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>0.433398</t>
+          <t>0.00312</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2806,12 +2794,12 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>0.437931</t>
+          <t>0.005541</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>0.000187</t>
+          <t>2.3e-05</t>
         </is>
       </c>
     </row>
@@ -2843,17 +2831,17 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>0.00236401</t>
+          <t>0.001546</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>8.8e-05</t>
+          <t>8.3e-05</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>0.330523</t>
+          <t>0.002215</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2863,12 +2851,12 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>0.334819</t>
+          <t>0.004954</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.6e-05</t>
         </is>
       </c>
     </row>
@@ -2900,19 +2888,19 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
+          <t>0.001722</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>7.9e-05</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
           <t>0.002419</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>9.4e-05</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>0.540015</t>
-        </is>
-      </c>
       <c r="I44" t="inlineStr">
         <is>
           <t>0</t>
@@ -2920,12 +2908,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>0.544399</t>
+          <t>0.005369</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2.9e-05</t>
+          <t>3.5e-05</t>
         </is>
       </c>
     </row>
@@ -2957,17 +2945,17 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0.00253301</t>
+          <t>0.001569</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>9.1e-05</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>0.318566</t>
+          <t>0.001981</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2977,12 +2965,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>0.323026</t>
+          <t>0.004807</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>3.5e-05</t>
+          <t>4.5e-05</t>
         </is>
       </c>
     </row>
@@ -3014,17 +3002,17 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>0.002313</t>
+          <t>0.003157</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.000134</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>0.477867</t>
+          <t>0.00766</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -3034,12 +3022,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>0.482196</t>
+          <t>0.01273</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>3.5e-05</t>
+          <t>6.2e-05</t>
         </is>
       </c>
     </row>
@@ -3071,17 +3059,17 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>0.002361</t>
+          <t>0.001721</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>9.9e-05</t>
+          <t>8.1e-05</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>0.53538</t>
+          <t>0.002284</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -3091,12 +3079,12 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>0.539919</t>
+          <t>0.005235</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.7e-05</t>
         </is>
       </c>
     </row>
@@ -3128,17 +3116,17 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>0.002236</t>
+          <t>0.001664</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>0.000108</t>
+          <t>7.7e-05</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>0.481045</t>
+          <t>0.001837</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3148,12 +3136,12 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>0.485323</t>
+          <t>0.004706</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>3.5e-05</t>
+          <t>3.6e-05</t>
         </is>
       </c>
     </row>
@@ -3185,17 +3173,17 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>0.002334</t>
+          <t>0.001746</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>9.1e-05</t>
+          <t>8.7e-05</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>0.455381</t>
+          <t>0.00186</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -3205,12 +3193,12 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>0.459688</t>
+          <t>0.004864</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>4.4e-05</t>
         </is>
       </c>
     </row>
@@ -3242,17 +3230,17 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>0.00253501</t>
+          <t>0.001651</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>9.2e-05</t>
+          <t>7.9e-05</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>0.374815</t>
+          <t>0.002024</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3262,12 +3250,12 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>0.379305</t>
+          <t>0.004963</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4e-05</t>
         </is>
       </c>
     </row>
@@ -3295,17 +3283,17 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>0.001867</t>
+          <t>0.001315</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>7.8e-05</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>0.475762</t>
+          <t>0.002234</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -3315,12 +3303,12 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>0.479547</t>
+          <t>0.004654</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>1.3e-05</t>
+          <t>1.7e-05</t>
         </is>
       </c>
     </row>
@@ -3352,17 +3340,17 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>0.00276601</t>
+          <t>0.001895</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>9.1e-05</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>0.459155</t>
+          <t>0.00184</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -3372,12 +3360,12 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>0.463907</t>
+          <t>0.00499</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>3.3e-05</t>
+          <t>3.4e-05</t>
         </is>
       </c>
     </row>
@@ -3409,17 +3397,17 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>0.00281401</t>
+          <t>0.001618</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>7.8e-05</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>0.525254</t>
+          <t>0.004727</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -3429,12 +3417,12 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>0.530085</t>
+          <t>0.007555</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>3.8e-05</t>
+          <t>4.4e-05</t>
         </is>
       </c>
     </row>
@@ -3466,17 +3454,17 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>0.002436</t>
+          <t>0.003363</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>0.000134</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>0.5713</t>
+          <t>0.003035</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -3486,12 +3474,12 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>0.575711</t>
+          <t>0.008414</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>3.4e-05</t>
+          <t>4.9e-05</t>
         </is>
       </c>
     </row>
@@ -3523,17 +3511,17 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>0.00259001</t>
+          <t>0.002748</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.000142</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>0.461279</t>
+          <t>0.011506</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -3543,12 +3531,12 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>0.46591</t>
+          <t>0.01603</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>4.9e-05</t>
         </is>
       </c>
     </row>
@@ -3580,17 +3568,17 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>0.002421</t>
+          <t>0.001722</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>9.8e-05</t>
+          <t>9e-05</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>0.580252</t>
+          <t>0.00262</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -3600,12 +3588,12 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>0.584657</t>
+          <t>0.005596</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>3.4e-05</t>
+          <t>3.7e-05</t>
         </is>
       </c>
     </row>
@@ -3637,17 +3625,17 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>0.002305</t>
+          <t>0.001709</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>9.6e-05</t>
+          <t>8.3e-05</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>0.411768</t>
+          <t>0.004549</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -3657,12 +3645,12 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>0.416056</t>
+          <t>0.007485</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>3.2e-05</t>
+          <t>3.5e-05</t>
         </is>
       </c>
     </row>
@@ -3694,17 +3682,17 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>0.00271101</t>
+          <t>0.001598</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>8.6e-05</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>0.438734</t>
+          <t>0.001913</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -3714,12 +3702,12 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>0.443456</t>
+          <t>0.004716</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -3751,17 +3739,17 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>0.002368</t>
+          <t>0.001649</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>7.9e-05</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>0.471642</t>
+          <t>0.004191</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -3771,12 +3759,12 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>0.475947</t>
+          <t>0.007073</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.8e-05</t>
         </is>
       </c>
     </row>
@@ -3808,17 +3796,17 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>0.00252801</t>
+          <t>0.00163</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>9.3e-05</t>
+          <t>9.1e-05</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>0.375232</t>
+          <t>0.006697</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -3828,12 +3816,12 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>0.379779</t>
+          <t>0.009589</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>4.1e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -3865,17 +3853,17 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>0.00279101</t>
+          <t>0.001625</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>0.000112</t>
+          <t>7.7e-05</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>0.446668</t>
+          <t>0.002322</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -3885,12 +3873,12 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>0.451531</t>
+          <t>0.005134</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>4e-05</t>
         </is>
       </c>
     </row>
@@ -3922,17 +3910,17 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>0.00277801</t>
+          <t>0.001644</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>0.000104</t>
+          <t>7.6e-05</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>0.362307</t>
+          <t>0.002133</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -3942,12 +3930,12 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>0.367129</t>
+          <t>0.004967</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>3e-05</t>
+          <t>3.7e-05</t>
         </is>
       </c>
     </row>
@@ -3979,17 +3967,17 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>0.002413</t>
+          <t>0.001723</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>0.000106</t>
+          <t>8e-05</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>0.432141</t>
+          <t>0.002503</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -3999,12 +3987,12 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>0.436555</t>
+          <t>0.00547</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.4e-05</t>
         </is>
       </c>
     </row>
@@ -4036,17 +4024,17 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>0.002378</t>
+          <t>0.001666</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>0.000109</t>
+          <t>8.7e-05</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>0.459591</t>
+          <t>0.004133</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -4056,12 +4044,12 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>0.464004</t>
+          <t>0.007067</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>3.8e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -4093,17 +4081,17 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>0.00267901</t>
+          <t>0.001617</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>7.7e-05</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>0.457852</t>
+          <t>0.002153</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -4113,12 +4101,12 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>0.462584</t>
+          <t>0.004971</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>3.4e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -4150,17 +4138,17 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>0.002269</t>
+          <t>0.001735</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>9.2e-05</t>
+          <t>8.5e-05</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>0.466607</t>
+          <t>0.00251</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -4170,12 +4158,12 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>0.470917</t>
+          <t>0.00552</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.5e-05</t>
         </is>
       </c>
     </row>
@@ -4207,17 +4195,17 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>0.002093</t>
+          <t>0.001557</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>9e-05</t>
+          <t>8.1e-05</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>0.346975</t>
+          <t>0.002726</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -4227,12 +4215,12 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>0.350976</t>
+          <t>0.005486</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.9e-05</t>
         </is>
       </c>
     </row>
@@ -4264,17 +4252,17 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>0.00259801</t>
+          <t>0.001652</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>8.2e-05</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>0.391993</t>
+          <t>0.001907</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
@@ -4284,12 +4272,12 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>0.396559</t>
+          <t>0.004816</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -4321,17 +4309,17 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>0.002288</t>
+          <t>0.001736</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>9.7e-05</t>
+          <t>8.7e-05</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>0.444289</t>
+          <t>0.00236</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -4341,12 +4329,12 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>0.44857</t>
+          <t>0.005341</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -4378,17 +4366,17 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>0.00262301</t>
+          <t>0.00162</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>9.5e-05</t>
+          <t>8.1e-05</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>0.401351</t>
+          <t>0.001682</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -4398,12 +4386,12 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>0.40609</t>
+          <t>0.004519</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -4435,17 +4423,17 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>0.00279301</t>
+          <t>0.001681</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>9.3e-05</t>
+          <t>8.6e-05</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>0.408387</t>
+          <t>0.000718</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -4455,12 +4443,12 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>0.413161</t>
+          <t>0.003605</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>3.2e-05</t>
+          <t>3.8e-05</t>
         </is>
       </c>
     </row>
@@ -4492,17 +4480,17 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>0.002348</t>
+          <t>0.001694</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>9.8e-05</t>
+          <t>8.2e-05</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>0.595488</t>
+          <t>0.00104</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -4512,12 +4500,12 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>0.599871</t>
+          <t>0.004022</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>3.2e-05</t>
+          <t>3.9e-05</t>
         </is>
       </c>
     </row>
@@ -4549,17 +4537,17 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>0.002378</t>
+          <t>0.00175</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>9.3e-05</t>
+          <t>7.9e-05</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>0.499339</t>
+          <t>0.001195</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -4569,12 +4557,12 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>0.503703</t>
+          <t>0.004198</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.6e-05</t>
         </is>
       </c>
     </row>
@@ -4606,17 +4594,17 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>0.00283101</t>
+          <t>0.00163</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>9e-05</t>
+          <t>7.6e-05</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>0.47355</t>
+          <t>0.001876</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -4626,12 +4614,12 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>0.478363</t>
+          <t>0.004707</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -4663,17 +4651,17 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>0.002398</t>
+          <t>0.001439</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>9.8e-05</t>
+          <t>8.5e-05</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>0.440272</t>
+          <t>0.004216</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -4683,12 +4671,12 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>0.445058</t>
+          <t>0.006889</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>0.000142</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -4720,17 +4708,17 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>0.00276301</t>
+          <t>0.001578</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>9.8e-05</t>
+          <t>7.8e-05</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>0.512205</t>
+          <t>0.003584</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -4740,7 +4728,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>0.516952</t>
+          <t>0.006326</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -4777,17 +4765,17 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>0.00290401</t>
+          <t>0.001646</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>0.000104</t>
+          <t>7.8e-05</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>0.595983</t>
+          <t>0.002661</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -4797,7 +4785,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>0.60094</t>
+          <t>0.005496</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -4834,17 +4822,17 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>0.00256801</t>
+          <t>0.001629</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>9e-05</t>
+          <t>7.8e-05</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>0.544843</t>
+          <t>0.00354</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -4854,12 +4842,12 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>0.549399</t>
+          <t>0.006392</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>3.4e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -4891,17 +4879,17 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>0.00266901</t>
+          <t>0.00159</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>8e-05</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>0.520465</t>
+          <t>0.003991</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -4911,12 +4899,12 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>0.525121</t>
+          <t>0.00675</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>3.9e-05</t>
         </is>
       </c>
     </row>
@@ -4948,17 +4936,17 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>0.002376</t>
+          <t>0.001713</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>9.1e-05</t>
+          <t>7.7e-05</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>0.49292</t>
+          <t>0.002144</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -4968,12 +4956,12 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>0.497333</t>
+          <t>0.0051</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>3.2e-05</t>
+          <t>3.3e-05</t>
         </is>
       </c>
     </row>
@@ -5005,17 +4993,17 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>0.00256401</t>
+          <t>0.001651</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>9.6e-05</t>
+          <t>7.7e-05</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>0.391681</t>
+          <t>0.001874</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -5025,12 +5013,12 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>0.396215</t>
+          <t>0.004756</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -5062,17 +5050,17 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>0.00297101</t>
+          <t>0.001652</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>0.000101</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>0.544326</t>
+          <t>0.005005</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
@@ -5082,12 +5070,12 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>0.549546</t>
+          <t>0.007905</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -5119,17 +5107,17 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>0.002571</t>
+          <t>0.001685</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>9.2e-05</t>
+          <t>7.9e-05</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>0.409413</t>
+          <t>0.003026</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -5139,12 +5127,12 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>0.413941</t>
+          <t>0.005917</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>3e-05</t>
+          <t>3.6e-05</t>
         </is>
       </c>
     </row>
@@ -5176,17 +5164,17 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>0.00281101</t>
+          <t>0.001603</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>9.3e-05</t>
+          <t>8.4e-05</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>0.389662</t>
+          <t>0.002068</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -5196,12 +5184,12 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>0.394629</t>
+          <t>0.004864</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>3.9e-05</t>
+          <t>4.5e-05</t>
         </is>
       </c>
     </row>
@@ -5233,17 +5221,17 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>0.00249501</t>
+          <t>0.00277</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>8.3e-05</t>
+          <t>0.000142</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>0.258311</t>
+          <t>0.004385</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -5253,12 +5241,12 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>0.26273</t>
+          <t>0.008952</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>3e-05</t>
+          <t>5.5e-05</t>
         </is>
       </c>
     </row>
@@ -5290,17 +5278,17 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>0.00252901</t>
+          <t>0.001631</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>8.2e-05</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>0.478673</t>
+          <t>0.002006</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -5310,12 +5298,12 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>0.48322</t>
+          <t>0.004881</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>4.1e-05</t>
         </is>
       </c>
     </row>
@@ -5347,17 +5335,17 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>0.002427</t>
+          <t>0.001742</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>8.5e-05</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>0.621141</t>
+          <t>0.003001</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
@@ -5367,12 +5355,12 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>0.625597</t>
+          <t>0.006006</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.5e-05</t>
         </is>
       </c>
     </row>
@@ -5404,17 +5392,17 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>0.002298</t>
+          <t>0.001708</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>9.9e-05</t>
+          <t>9e-05</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>0.463425</t>
+          <t>0.002134</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -5424,12 +5412,12 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>0.4677</t>
+          <t>0.005108</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.5e-05</t>
         </is>
       </c>
     </row>
@@ -5461,17 +5449,17 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>0.002357</t>
+          <t>0.001731</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>9e-05</t>
+          <t>7.6e-05</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>0.491197</t>
+          <t>0.002557</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -5481,12 +5469,12 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>0.495517</t>
+          <t>0.005515</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>3.3e-05</t>
+          <t>3.6e-05</t>
         </is>
       </c>
     </row>
@@ -5514,17 +5502,17 @@
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
         <is>
-          <t>0.002146</t>
+          <t>0.001282</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>8.5e-05</t>
+          <t>8.2e-05</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>0.345623</t>
+          <t>0.002521</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -5534,12 +5522,12 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>0.349734</t>
+          <t>0.004978</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>1.3e-05</t>
+          <t>2e-05</t>
         </is>
       </c>
     </row>
@@ -5571,17 +5559,17 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>0.00270101</t>
+          <t>0.001689</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>8.7e-05</t>
+          <t>8.2e-05</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>0.430209</t>
+          <t>0.001247</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
@@ -5591,12 +5579,12 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>0.434885</t>
+          <t>0.004161</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>3.1e-05</t>
+          <t>3.4e-05</t>
         </is>
       </c>
     </row>
@@ -5628,17 +5616,17 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>0.00256601</t>
+          <t>0.001676</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>9.9e-05</t>
+          <t>8.5e-05</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>0.467333</t>
+          <t>0.001037</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
@@ -5648,12 +5636,12 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>0.471858</t>
+          <t>0.003919</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>3.4e-05</t>
+          <t>3.6e-05</t>
         </is>
       </c>
     </row>
@@ -5685,17 +5673,17 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>0.002254</t>
+          <t>0.001617</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>9.2e-05</t>
+          <t>7.6e-05</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>0.541918</t>
+          <t>0.002238</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -5705,12 +5693,12 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>0.546116</t>
+          <t>0.005095</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>3.8e-05</t>
         </is>
       </c>
     </row>
@@ -5742,17 +5730,17 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>0.002418</t>
+          <t>0.001714</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>9.5e-05</t>
+          <t>8.5e-05</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>0.556663</t>
+          <t>0.001642</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
@@ -5762,12 +5750,12 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>0.561241</t>
+          <t>0.004621</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>3.4e-05</t>
+          <t>4.3e-05</t>
         </is>
       </c>
     </row>
@@ -5799,17 +5787,17 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>0.002144</t>
+          <t>0.001407</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>9e-05</t>
+          <t>8.1e-05</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>0.385199</t>
+          <t>0.002955</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -5819,12 +5807,12 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>0.389393</t>
+          <t>0.005564</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>4.7e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -5856,17 +5844,17 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>0.00271601</t>
+          <t>0.001636</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>9.8e-05</t>
+          <t>8.3e-05</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>0.476487</t>
+          <t>0.00522</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
@@ -5876,12 +5864,12 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>0.481179</t>
+          <t>0.008083</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>3.5e-05</t>
+          <t>3.9e-05</t>
         </is>
       </c>
     </row>
@@ -5913,17 +5901,17 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>0.002283</t>
+          <t>0.001623</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>9.9e-05</t>
+          <t>0.000103</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>0.533699</t>
+          <t>0.006879</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -5933,12 +5921,12 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>0.537935</t>
+          <t>0.009798</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -5970,17 +5958,17 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>0.00229</t>
+          <t>0.001651</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>9.7e-05</t>
+          <t>9.1e-05</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>0.46167</t>
+          <t>0.004178</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
@@ -5990,12 +5978,12 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>0.465901</t>
+          <t>0.007105</t>
         </is>
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>3.7e-05</t>
+          <t>4.2e-05</t>
         </is>
       </c>
     </row>
@@ -6027,17 +6015,17 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>0.00260501</t>
+          <t>0.001664</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>9.4e-05</t>
+          <t>8.6e-05</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>0.397637</t>
+          <t>0.001684</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -6047,12 +6035,12 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>0.402192</t>
+          <t>0.004599</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.6e-05</t>
         </is>
       </c>
     </row>
@@ -6084,17 +6072,17 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>0.00240101</t>
+          <t>0.001561</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>8.9e-05</t>
+          <t>8.8e-05</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>0.31955</t>
+          <t>0.001921</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
@@ -6104,12 +6092,12 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>0.323919</t>
+          <t>0.004751</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>3.6e-05</t>
+          <t>4.8e-05</t>
         </is>
       </c>
     </row>
@@ -6141,17 +6129,17 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>0.00248301</t>
+          <t>0.001561</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>8.9e-05</t>
+          <t>8.8e-05</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>0.388999</t>
+          <t>0.005074</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
@@ -6161,12 +6149,12 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>0.393674</t>
+          <t>0.007896</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>3.4e-05</t>
+          <t>4.5e-05</t>
         </is>
       </c>
     </row>

</xml_diff>